<commit_message>
step 0 is complete
</commit_message>
<xml_diff>
--- a/bot_outputs/step_0_out.xlsx
+++ b/bot_outputs/step_0_out.xlsx
@@ -8,7 +8,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$N$221</definedName>
+  </definedNames>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -406,7 +408,8 @@
   <dimension ref="A1:N221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -467,7 +470,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Volumes</t>
+          <t>Volumes:</t>
         </is>
       </c>
     </row>
@@ -671,7 +674,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Revenue:</t>
         </is>
       </c>
     </row>
@@ -971,7 +974,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating Expenses:</t>
         </is>
       </c>
     </row>
@@ -2471,7 +2474,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Volumes</t>
+          <t>Volumes:</t>
         </is>
       </c>
     </row>
@@ -2675,7 +2678,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Revenue:</t>
         </is>
       </c>
     </row>
@@ -2975,7 +2978,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating Expenses:</t>
         </is>
       </c>
     </row>
@@ -4475,7 +4478,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Volumes</t>
+          <t>Volumes:</t>
         </is>
       </c>
     </row>
@@ -4679,7 +4682,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Revenue:</t>
         </is>
       </c>
     </row>
@@ -4979,7 +4982,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating Expenses:</t>
         </is>
       </c>
     </row>
@@ -6479,7 +6482,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Volumes</t>
+          <t>Volumes:</t>
         </is>
       </c>
     </row>
@@ -6683,7 +6686,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Revenue:</t>
         </is>
       </c>
     </row>
@@ -6983,7 +6986,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating Expenses:</t>
         </is>
       </c>
     </row>
@@ -8483,7 +8486,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Volumes</t>
+          <t>Volumes:</t>
         </is>
       </c>
     </row>
@@ -8687,7 +8690,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Revenue:</t>
         </is>
       </c>
     </row>
@@ -8987,7 +8990,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating Expenses:</t>
         </is>
       </c>
     </row>
@@ -10480,6 +10483,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N221"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
step 1 is complete
</commit_message>
<xml_diff>
--- a/bot_outputs/step_0_out.xlsx
+++ b/bot_outputs/step_0_out.xlsx
@@ -6,10 +6,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Example0gross_LOS" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$N$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Example0gross_LOS'!$A$1:$N$221</definedName>
   </definedNames>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>